<commit_message>
Re-upload breakoutboard Excel file
hope to make formatting problem go away
</commit_message>
<xml_diff>
--- a/input/BrkOutBrd_Pin_Assignments_Mar27_2018_PM1.xlsx
+++ b/input/BrkOutBrd_Pin_Assignments_Mar27_2018_PM1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UT\Backplane-Remapping\Pathfinder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yzs\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB2CBBC-BDB7-4CFE-A509-8E6C97D9286F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11610"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PinAssignments" sheetId="1" r:id="rId1"/>
@@ -2430,7 +2431,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2674,7 +2675,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2979,25 +2986,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.140625" customWidth="1"/>
-    <col min="4" max="4" width="29.140625" customWidth="1"/>
-    <col min="5" max="5" width="4.42578125" customWidth="1"/>
-    <col min="6" max="6" width="31.7109375" customWidth="1"/>
+    <col min="1" max="1" width="33.1796875" customWidth="1"/>
+    <col min="4" max="4" width="29.1796875" customWidth="1"/>
+    <col min="5" max="5" width="4.453125" customWidth="1"/>
+    <col min="6" max="6" width="31.7265625" customWidth="1"/>
     <col min="9" max="9" width="32" customWidth="1"/>
-    <col min="10" max="10" width="4.42578125" customWidth="1"/>
-    <col min="11" max="11" width="31.85546875" customWidth="1"/>
+    <col min="10" max="10" width="4.453125" customWidth="1"/>
+    <col min="11" max="11" width="31.81640625" customWidth="1"/>
     <col min="14" max="14" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3005,12 +3012,12 @@
         <v>767</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -3050,7 +3057,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>13</v>
       </c>
@@ -3090,7 +3097,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>23</v>
       </c>
@@ -3128,7 +3135,7 @@
       </c>
       <c r="N6" s="13"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>33</v>
       </c>
@@ -3166,7 +3173,7 @@
       </c>
       <c r="N7" s="13"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
         <v>43</v>
       </c>
@@ -3204,7 +3211,7 @@
       </c>
       <c r="N8" s="13"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>53</v>
       </c>
@@ -3242,7 +3249,7 @@
       </c>
       <c r="N9" s="13"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>64</v>
       </c>
@@ -3278,7 +3285,7 @@
       </c>
       <c r="N10" s="13"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>74</v>
       </c>
@@ -3314,7 +3321,7 @@
       </c>
       <c r="N11" s="13"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
         <v>84</v>
       </c>
@@ -3350,7 +3357,7 @@
       </c>
       <c r="N12" s="13"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>5</v>
       </c>
@@ -3386,7 +3393,7 @@
       </c>
       <c r="N13" s="13"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="s">
         <v>102</v>
       </c>
@@ -3422,7 +3429,7 @@
       </c>
       <c r="N14" s="13"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="14" t="s">
         <v>109</v>
       </c>
@@ -3462,7 +3469,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
         <v>118</v>
       </c>
@@ -3502,7 +3509,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
         <v>127</v>
       </c>
@@ -3540,7 +3547,7 @@
       </c>
       <c r="N17" s="13"/>
     </row>
-    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="18" t="s">
         <v>135</v>
       </c>
@@ -3578,7 +3585,7 @@
       </c>
       <c r="N18" s="13"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E19" s="6"/>
       <c r="J19" s="6"/>
       <c r="K19" s="16" t="s">
@@ -3592,7 +3599,7 @@
       </c>
       <c r="N19" s="13"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E20" s="6"/>
       <c r="J20" s="6"/>
       <c r="K20" s="16" t="s">
@@ -3606,7 +3613,7 @@
       </c>
       <c r="N20" s="13"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E21" s="6"/>
       <c r="J21" s="6"/>
       <c r="K21" s="16" t="s">
@@ -3620,7 +3627,7 @@
       </c>
       <c r="N21" s="13"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E22" s="6"/>
       <c r="J22" s="6"/>
       <c r="K22" s="16" t="s">
@@ -3634,7 +3641,7 @@
       </c>
       <c r="N22" s="13"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E23" s="6"/>
       <c r="J23" s="6"/>
       <c r="K23" s="16" t="s">
@@ -3648,7 +3655,7 @@
       </c>
       <c r="N23" s="13"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E24" s="6"/>
       <c r="J24" s="6"/>
       <c r="K24" s="16" t="s">
@@ -3662,7 +3669,7 @@
       </c>
       <c r="N24" s="13"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E25" s="6"/>
       <c r="J25" s="6"/>
       <c r="K25" s="16" t="s">
@@ -3676,7 +3683,7 @@
       </c>
       <c r="N25" s="13"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="16" t="s">
@@ -3690,7 +3697,7 @@
       </c>
       <c r="N26" s="13"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E27" s="6"/>
       <c r="J27" s="6"/>
       <c r="K27" s="16" t="s">
@@ -3704,7 +3711,7 @@
       </c>
       <c r="N27" s="13"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E28" s="6"/>
       <c r="J28" s="6"/>
       <c r="K28" s="16" t="s">
@@ -3718,7 +3725,7 @@
       </c>
       <c r="N28" s="13"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E29" s="6"/>
       <c r="J29" s="6"/>
       <c r="K29" s="16" t="s">
@@ -3732,7 +3739,7 @@
       </c>
       <c r="N29" s="13"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E30" s="6"/>
       <c r="J30" s="6"/>
       <c r="K30" s="16" t="s">
@@ -3746,7 +3753,7 @@
       </c>
       <c r="N30" s="13"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E31" s="6"/>
       <c r="J31" s="6"/>
       <c r="K31" s="16" t="s">
@@ -3760,7 +3767,7 @@
       </c>
       <c r="N31" s="13"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E32" s="6"/>
       <c r="J32" s="6"/>
       <c r="K32" s="16" t="s">
@@ -3774,7 +3781,7 @@
       </c>
       <c r="N32" s="13"/>
     </row>
-    <row r="33" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E33" s="6"/>
       <c r="J33" s="6"/>
       <c r="K33" s="16" t="s">
@@ -3788,7 +3795,7 @@
       </c>
       <c r="N33" s="13"/>
     </row>
-    <row r="34" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E34" s="6"/>
       <c r="J34" s="6"/>
       <c r="K34" s="16" t="s">
@@ -3802,7 +3809,7 @@
       </c>
       <c r="N34" s="13"/>
     </row>
-    <row r="35" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E35" s="6"/>
       <c r="J35" s="6"/>
       <c r="K35" s="16" t="s">
@@ -3816,7 +3823,7 @@
       </c>
       <c r="N35" s="13"/>
     </row>
-    <row r="36" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E36" s="6"/>
       <c r="J36" s="6"/>
       <c r="K36" s="16" t="s">
@@ -3830,7 +3837,7 @@
       </c>
       <c r="N36" s="13"/>
     </row>
-    <row r="37" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E37" s="6"/>
       <c r="J37" s="6"/>
       <c r="K37" s="16" t="s">
@@ -3844,7 +3851,7 @@
       </c>
       <c r="N37" s="13"/>
     </row>
-    <row r="38" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E38" s="6"/>
       <c r="J38" s="6"/>
       <c r="K38" s="16" t="s">
@@ -3858,7 +3865,7 @@
       </c>
       <c r="N38" s="13"/>
     </row>
-    <row r="39" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E39" s="6"/>
       <c r="J39" s="6"/>
       <c r="K39" s="16" t="s">
@@ -3872,7 +3879,7 @@
       </c>
       <c r="N39" s="13"/>
     </row>
-    <row r="40" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E40" s="6"/>
       <c r="J40" s="6"/>
       <c r="K40" s="16" t="s">
@@ -3886,7 +3893,7 @@
       </c>
       <c r="N40" s="13"/>
     </row>
-    <row r="41" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E41" s="6"/>
       <c r="J41" s="6"/>
       <c r="K41" s="16" t="s">
@@ -3900,7 +3907,7 @@
       </c>
       <c r="N41" s="13"/>
     </row>
-    <row r="42" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E42" s="6"/>
       <c r="J42" s="6"/>
       <c r="K42" s="16" t="s">
@@ -3914,7 +3921,7 @@
       </c>
       <c r="N42" s="13"/>
     </row>
-    <row r="43" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E43" s="6"/>
       <c r="J43" s="6"/>
       <c r="K43" s="16"/>
@@ -3926,7 +3933,7 @@
       </c>
       <c r="N43" s="13"/>
     </row>
-    <row r="44" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E44" s="6"/>
       <c r="J44" s="6"/>
       <c r="K44" s="16"/>
@@ -3938,7 +3945,7 @@
       </c>
       <c r="N44" s="13"/>
     </row>
-    <row r="45" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E45" s="6"/>
       <c r="J45" s="6"/>
       <c r="K45" s="16"/>
@@ -3950,7 +3957,7 @@
       </c>
       <c r="N45" s="13"/>
     </row>
-    <row r="46" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E46" s="6"/>
       <c r="J46" s="6"/>
       <c r="K46" s="16"/>
@@ -3962,7 +3969,7 @@
       </c>
       <c r="N46" s="13"/>
     </row>
-    <row r="47" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E47" s="6"/>
       <c r="J47" s="6"/>
       <c r="K47" s="16"/>
@@ -3974,7 +3981,7 @@
       </c>
       <c r="N47" s="13"/>
     </row>
-    <row r="48" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E48" s="6"/>
       <c r="J48" s="6"/>
       <c r="K48" s="16" t="s">
@@ -3988,7 +3995,7 @@
       </c>
       <c r="N48" s="13"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E49" s="6"/>
       <c r="J49" s="6"/>
       <c r="K49" s="16" t="s">
@@ -4002,7 +4009,7 @@
       </c>
       <c r="N49" s="13"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E50" s="6"/>
       <c r="J50" s="6"/>
       <c r="K50" s="16" t="s">
@@ -4016,7 +4023,7 @@
       </c>
       <c r="N50" s="13"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E51" s="6"/>
       <c r="J51" s="6"/>
       <c r="K51" s="16" t="s">
@@ -4030,7 +4037,7 @@
       </c>
       <c r="N51" s="13"/>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E52" s="6"/>
       <c r="J52" s="6"/>
       <c r="K52" s="16" t="s">
@@ -4046,7 +4053,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E53" s="6"/>
       <c r="F53" s="21"/>
       <c r="G53" s="21"/>
@@ -4066,7 +4073,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="24"/>
       <c r="B54" s="24"/>
       <c r="C54" s="24"/>
@@ -4082,7 +4089,7 @@
       <c r="M54" s="24"/>
       <c r="N54" s="24"/>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A55" s="7" t="s">
         <v>243</v>
       </c>
@@ -4122,7 +4129,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A56" s="14" t="s">
         <v>253</v>
       </c>
@@ -4162,7 +4169,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A57" s="14" t="s">
         <v>263</v>
       </c>
@@ -4200,7 +4207,7 @@
       </c>
       <c r="N57" s="13"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A58" s="14" t="s">
         <v>273</v>
       </c>
@@ -4240,7 +4247,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A59" s="14" t="s">
         <v>283</v>
       </c>
@@ -4280,7 +4287,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A60" s="14" t="s">
         <v>293</v>
       </c>
@@ -4318,7 +4325,7 @@
       </c>
       <c r="N60" s="13"/>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A61" s="14" t="s">
         <v>304</v>
       </c>
@@ -4356,7 +4363,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A62" s="14" t="s">
         <v>314</v>
       </c>
@@ -4396,7 +4403,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A63" s="14" t="s">
         <v>325</v>
       </c>
@@ -4434,7 +4441,7 @@
       </c>
       <c r="N63" s="13"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A64" s="14" t="s">
         <v>336</v>
       </c>
@@ -4474,7 +4481,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A65" s="14" t="s">
         <v>347</v>
       </c>
@@ -4514,7 +4521,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A66" s="14" t="s">
         <v>357</v>
       </c>
@@ -4552,7 +4559,7 @@
       </c>
       <c r="N66" s="13"/>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A67" s="14" t="s">
         <v>367</v>
       </c>
@@ -4592,7 +4599,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A68" s="14" t="s">
         <v>377</v>
       </c>
@@ -4632,7 +4639,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" s="18" t="s">
         <v>387</v>
       </c>
@@ -4670,7 +4677,7 @@
       </c>
       <c r="N69" s="17"/>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E70" s="6"/>
       <c r="J70" s="6"/>
       <c r="K70" s="16" t="s">
@@ -4686,7 +4693,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E71" s="6"/>
       <c r="J71" s="6"/>
       <c r="K71" s="16" t="s">
@@ -4702,7 +4709,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E72" s="6"/>
       <c r="J72" s="6"/>
       <c r="K72" s="16" t="s">
@@ -4716,7 +4723,7 @@
       </c>
       <c r="N72" s="13"/>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E73" s="6"/>
       <c r="J73" s="6"/>
       <c r="K73" s="16" t="s">
@@ -4730,7 +4737,7 @@
       </c>
       <c r="N73" s="13"/>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E74" s="6"/>
       <c r="J74" s="6"/>
       <c r="K74" s="16" t="s">
@@ -4744,7 +4751,7 @@
       </c>
       <c r="N74" s="13"/>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E75" s="6"/>
       <c r="J75" s="6"/>
       <c r="K75" s="16" t="s">
@@ -4758,7 +4765,7 @@
       </c>
       <c r="N75" s="13"/>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E76" s="6"/>
       <c r="G76" s="21"/>
       <c r="H76" s="21"/>
@@ -4774,7 +4781,7 @@
       </c>
       <c r="N76" s="13"/>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E77" s="6"/>
       <c r="H77" s="21"/>
       <c r="J77" s="6"/>
@@ -4789,7 +4796,7 @@
       </c>
       <c r="N77" s="13"/>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E78" s="6"/>
       <c r="G78" s="21"/>
       <c r="H78" s="21"/>
@@ -4805,7 +4812,7 @@
       </c>
       <c r="N78" s="13"/>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E79" s="6"/>
       <c r="H79" s="21"/>
       <c r="J79" s="6"/>
@@ -4820,7 +4827,7 @@
       </c>
       <c r="N79" s="13"/>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E80" s="6"/>
       <c r="G80" s="21"/>
       <c r="H80" s="21"/>
@@ -4836,7 +4843,7 @@
       </c>
       <c r="N80" s="13"/>
     </row>
-    <row r="81" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E81" s="6"/>
       <c r="H81" s="21"/>
       <c r="J81" s="6"/>
@@ -4851,7 +4858,7 @@
       </c>
       <c r="N81" s="13"/>
     </row>
-    <row r="82" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E82" s="6"/>
       <c r="G82" s="21"/>
       <c r="H82" s="21"/>
@@ -4867,7 +4874,7 @@
       </c>
       <c r="N82" s="13"/>
     </row>
-    <row r="83" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E83" s="6"/>
       <c r="H83" s="21"/>
       <c r="J83" s="6"/>
@@ -4882,7 +4889,7 @@
       </c>
       <c r="N83" s="13"/>
     </row>
-    <row r="84" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E84" s="6"/>
       <c r="G84" s="21"/>
       <c r="H84" s="21"/>
@@ -4898,7 +4905,7 @@
       </c>
       <c r="N84" s="13"/>
     </row>
-    <row r="85" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E85" s="6"/>
       <c r="H85" s="21"/>
       <c r="J85" s="6"/>
@@ -4913,7 +4920,7 @@
       </c>
       <c r="N85" s="13"/>
     </row>
-    <row r="86" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E86" s="6"/>
       <c r="G86" s="21"/>
       <c r="H86" s="21"/>
@@ -4929,7 +4936,7 @@
       </c>
       <c r="N86" s="13"/>
     </row>
-    <row r="87" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E87" s="6"/>
       <c r="J87" s="6"/>
       <c r="K87" s="16" t="s">
@@ -4943,7 +4950,7 @@
       </c>
       <c r="N87" s="13"/>
     </row>
-    <row r="88" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E88" s="6"/>
       <c r="G88" s="21"/>
       <c r="J88" s="6"/>
@@ -4958,7 +4965,7 @@
       </c>
       <c r="N88" s="13"/>
     </row>
-    <row r="89" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E89" s="6"/>
       <c r="J89" s="6"/>
       <c r="K89" s="16" t="s">
@@ -4972,7 +4979,7 @@
       </c>
       <c r="N89" s="13"/>
     </row>
-    <row r="90" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E90" s="6"/>
       <c r="G90" s="21"/>
       <c r="J90" s="6"/>
@@ -4987,7 +4994,7 @@
       </c>
       <c r="N90" s="13"/>
     </row>
-    <row r="91" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E91" s="6"/>
       <c r="J91" s="6"/>
       <c r="K91" s="16" t="s">
@@ -5001,7 +5008,7 @@
       </c>
       <c r="N91" s="13"/>
     </row>
-    <row r="92" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E92" s="6"/>
       <c r="G92" s="21"/>
       <c r="J92" s="6"/>
@@ -5016,7 +5023,7 @@
       </c>
       <c r="N92" s="13"/>
     </row>
-    <row r="93" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E93" s="6"/>
       <c r="J93" s="6"/>
       <c r="K93" s="16" t="s">
@@ -5030,7 +5037,7 @@
       </c>
       <c r="N93" s="17"/>
     </row>
-    <row r="94" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E94" s="6"/>
       <c r="J94" s="6"/>
       <c r="K94" s="16" t="s">
@@ -5044,7 +5051,7 @@
       </c>
       <c r="N94" s="13"/>
     </row>
-    <row r="95" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E95" s="6"/>
       <c r="J95" s="6"/>
       <c r="K95" s="16" t="s">
@@ -5058,7 +5065,7 @@
       </c>
       <c r="N95" s="13"/>
     </row>
-    <row r="96" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E96" s="6"/>
       <c r="J96" s="6"/>
       <c r="K96" s="16" t="s">
@@ -5072,7 +5079,7 @@
       </c>
       <c r="N96" s="17"/>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E97" s="6"/>
       <c r="J97" s="6"/>
       <c r="K97" s="16" t="s">
@@ -5086,7 +5093,7 @@
       </c>
       <c r="N97" s="13"/>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E98" s="6"/>
       <c r="J98" s="6"/>
       <c r="K98" s="16"/>
@@ -5098,7 +5105,7 @@
       </c>
       <c r="N98" s="13"/>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E99" s="6"/>
       <c r="J99" s="6"/>
       <c r="K99" s="16" t="s">
@@ -5112,7 +5119,7 @@
       </c>
       <c r="N99" s="13"/>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E100" s="6"/>
       <c r="J100" s="6"/>
       <c r="K100" s="16" t="s">
@@ -5126,7 +5133,7 @@
       </c>
       <c r="N100" s="13"/>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E101" s="6"/>
       <c r="J101" s="6"/>
       <c r="K101" s="16" t="s">
@@ -5142,7 +5149,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E102" s="6"/>
       <c r="J102" s="6"/>
       <c r="K102" s="16" t="s">
@@ -5158,7 +5165,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E103" s="6"/>
       <c r="J103" s="6"/>
       <c r="K103" s="16" t="s">
@@ -5174,7 +5181,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="104" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E104" s="6"/>
       <c r="J104" s="6"/>
       <c r="K104" s="22" t="s">
@@ -5190,7 +5197,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A105" s="6"/>
       <c r="B105" s="6"/>
       <c r="C105" s="6"/>
@@ -5206,7 +5213,7 @@
       <c r="M105" s="6"/>
       <c r="N105" s="6"/>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A106" s="7" t="s">
         <v>505</v>
       </c>
@@ -5246,7 +5253,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A107" s="14" t="s">
         <v>515</v>
       </c>
@@ -5286,7 +5293,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A108" s="14" t="s">
         <v>525</v>
       </c>
@@ -5324,7 +5331,7 @@
       </c>
       <c r="N108" s="13"/>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A109" s="14" t="s">
         <v>535</v>
       </c>
@@ -5364,7 +5371,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A110" s="14" t="s">
         <v>545</v>
       </c>
@@ -5404,7 +5411,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A111" s="14" t="s">
         <v>555</v>
       </c>
@@ -5442,7 +5449,7 @@
       </c>
       <c r="N111" s="13"/>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A112" s="14" t="s">
         <v>566</v>
       </c>
@@ -5480,7 +5487,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A113" s="14" t="s">
         <v>576</v>
       </c>
@@ -5520,7 +5527,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A114" s="14" t="s">
         <v>587</v>
       </c>
@@ -5558,7 +5565,7 @@
       </c>
       <c r="N114" s="13"/>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A115" s="14" t="s">
         <v>598</v>
       </c>
@@ -5598,7 +5605,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A116" s="14" t="s">
         <v>609</v>
       </c>
@@ -5638,7 +5645,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A117" s="14" t="s">
         <v>619</v>
       </c>
@@ -5676,7 +5683,7 @@
       </c>
       <c r="N117" s="13"/>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A118" s="14" t="s">
         <v>629</v>
       </c>
@@ -5716,7 +5723,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A119" s="14" t="s">
         <v>639</v>
       </c>
@@ -5756,7 +5763,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A120" s="18" t="s">
         <v>649</v>
       </c>
@@ -5794,7 +5801,7 @@
       </c>
       <c r="N120" s="13"/>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E121" s="6"/>
       <c r="J121" s="6"/>
       <c r="K121" s="16" t="s">
@@ -5810,7 +5817,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E122" s="6"/>
       <c r="J122" s="6"/>
       <c r="K122" s="16" t="s">
@@ -5826,7 +5833,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E123" s="6"/>
       <c r="J123" s="6"/>
       <c r="K123" s="16" t="s">
@@ -5840,7 +5847,7 @@
       </c>
       <c r="N123" s="13"/>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E124" s="6"/>
       <c r="F124" s="26"/>
       <c r="G124" s="21"/>
@@ -5859,7 +5866,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E125" s="6"/>
       <c r="G125" s="21"/>
       <c r="H125" s="21"/>
@@ -5877,7 +5884,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E126" s="6"/>
       <c r="G126" s="21"/>
       <c r="H126" s="21"/>
@@ -5893,7 +5900,7 @@
       </c>
       <c r="N126" s="13"/>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E127" s="6"/>
       <c r="G127" s="21"/>
       <c r="H127" s="21"/>
@@ -5911,7 +5918,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E128" s="6"/>
       <c r="G128" s="21"/>
       <c r="H128" s="21"/>
@@ -5929,7 +5936,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="129" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="129" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E129" s="6"/>
       <c r="G129" s="21"/>
       <c r="H129" s="21"/>
@@ -5945,7 +5952,7 @@
       </c>
       <c r="N129" s="13"/>
     </row>
-    <row r="130" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="130" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E130" s="6"/>
       <c r="G130" s="21"/>
       <c r="H130" s="21"/>
@@ -5961,7 +5968,7 @@
       </c>
       <c r="N130" s="13"/>
     </row>
-    <row r="131" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="131" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E131" s="6"/>
       <c r="G131" s="21"/>
       <c r="H131" s="21"/>
@@ -5977,7 +5984,7 @@
       </c>
       <c r="N131" s="13"/>
     </row>
-    <row r="132" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="132" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E132" s="6"/>
       <c r="G132" s="21"/>
       <c r="H132" s="21"/>
@@ -5993,7 +6000,7 @@
       </c>
       <c r="N132" s="13"/>
     </row>
-    <row r="133" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="133" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E133" s="6"/>
       <c r="G133" s="21"/>
       <c r="H133" s="21"/>
@@ -6009,7 +6016,7 @@
       </c>
       <c r="N133" s="13"/>
     </row>
-    <row r="134" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="134" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E134" s="6"/>
       <c r="G134" s="21"/>
       <c r="H134" s="21"/>
@@ -6025,7 +6032,7 @@
       </c>
       <c r="N134" s="13"/>
     </row>
-    <row r="135" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="135" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E135" s="6"/>
       <c r="G135" s="21"/>
       <c r="H135" s="21"/>
@@ -6041,7 +6048,7 @@
       </c>
       <c r="N135" s="13"/>
     </row>
-    <row r="136" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="136" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E136" s="6"/>
       <c r="G136" s="21"/>
       <c r="H136" s="21"/>
@@ -6057,7 +6064,7 @@
       </c>
       <c r="N136" s="13"/>
     </row>
-    <row r="137" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="137" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E137" s="6"/>
       <c r="G137" s="21"/>
       <c r="H137" s="21"/>
@@ -6073,7 +6080,7 @@
       </c>
       <c r="N137" s="13"/>
     </row>
-    <row r="138" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="138" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E138" s="6"/>
       <c r="G138" s="21"/>
       <c r="H138" s="21"/>
@@ -6089,7 +6096,7 @@
       </c>
       <c r="N138" s="13"/>
     </row>
-    <row r="139" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="139" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E139" s="6"/>
       <c r="J139" s="6"/>
       <c r="K139" s="16" t="s">
@@ -6103,7 +6110,7 @@
       </c>
       <c r="N139" s="13"/>
     </row>
-    <row r="140" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="140" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E140" s="6"/>
       <c r="J140" s="6"/>
       <c r="K140" s="16" t="s">
@@ -6117,7 +6124,7 @@
       </c>
       <c r="N140" s="13"/>
     </row>
-    <row r="141" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="141" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E141" s="6"/>
       <c r="J141" s="6"/>
       <c r="K141" s="16" t="s">
@@ -6131,7 +6138,7 @@
       </c>
       <c r="N141" s="13"/>
     </row>
-    <row r="142" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="142" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E142" s="6"/>
       <c r="J142" s="6"/>
       <c r="K142" s="16" t="s">
@@ -6145,7 +6152,7 @@
       </c>
       <c r="N142" s="13"/>
     </row>
-    <row r="143" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="143" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E143" s="6"/>
       <c r="J143" s="6"/>
       <c r="K143" s="16" t="s">
@@ -6159,7 +6166,7 @@
       </c>
       <c r="N143" s="13"/>
     </row>
-    <row r="144" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="144" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E144" s="6"/>
       <c r="J144" s="6"/>
       <c r="K144" s="16" t="s">
@@ -6173,7 +6180,7 @@
       </c>
       <c r="N144" s="13"/>
     </row>
-    <row r="145" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="145" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E145" s="6"/>
       <c r="J145" s="6"/>
       <c r="K145" s="16" t="s">
@@ -6187,7 +6194,7 @@
       </c>
       <c r="N145" s="13"/>
     </row>
-    <row r="146" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="146" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E146" s="6"/>
       <c r="J146" s="6"/>
       <c r="K146" s="16" t="s">
@@ -6201,7 +6208,7 @@
       </c>
       <c r="N146" s="13"/>
     </row>
-    <row r="147" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="147" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E147" s="6"/>
       <c r="J147" s="6"/>
       <c r="K147" s="16" t="s">
@@ -6215,7 +6222,7 @@
       </c>
       <c r="N147" s="13"/>
     </row>
-    <row r="148" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="148" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E148" s="6"/>
       <c r="J148" s="6"/>
       <c r="K148" s="16" t="s">
@@ -6229,7 +6236,7 @@
       </c>
       <c r="N148" s="13"/>
     </row>
-    <row r="149" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="149" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E149" s="6"/>
       <c r="J149" s="6"/>
       <c r="K149" s="16"/>
@@ -6241,7 +6248,7 @@
       </c>
       <c r="N149" s="13"/>
     </row>
-    <row r="150" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="150" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E150" s="6"/>
       <c r="J150" s="6"/>
       <c r="K150" s="16" t="s">
@@ -6255,7 +6262,7 @@
       </c>
       <c r="N150" s="13"/>
     </row>
-    <row r="151" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="151" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E151" s="6"/>
       <c r="J151" s="6"/>
       <c r="K151" s="16" t="s">
@@ -6269,7 +6276,7 @@
       </c>
       <c r="N151" s="13"/>
     </row>
-    <row r="152" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="152" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E152" s="6"/>
       <c r="J152" s="6"/>
       <c r="K152" s="16" t="s">
@@ -6285,7 +6292,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="153" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="153" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E153" s="6"/>
       <c r="J153" s="6"/>
       <c r="K153" s="16" t="s">
@@ -6301,7 +6308,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="154" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="154" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E154" s="6"/>
       <c r="J154" s="6"/>
       <c r="K154" s="16" t="s">
@@ -6317,7 +6324,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="155" spans="5:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E155" s="6"/>
       <c r="J155" s="6"/>
       <c r="K155" s="22" t="s">
@@ -6339,14 +6346,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
       <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>